<commit_message>
Refactor comment migration logic and add reply handling in threaded comments
</commit_message>
<xml_diff>
--- a/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
+++ b/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\darrenwest-allocate\openapi-2-excel\src\openapi2excel.tests\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF79B2DB-0F68-4191-8F27-DFE8054D1EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920F62B-A3A7-43F5-BDDB-FB2B621CE1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,13 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    A comment about a description
+    A comment about a description that becomes a discussion
 Reply:
-    A threaded reply where there is more infomation</t>
+    A threaded reply where there is more infomation
+Reply:
+    And continued input for long thread
+Reply:
+    This is the end of the discussion</t>
       </text>
     </comment>
     <comment ref="A12" authorId="1" shapeId="0" xr:uid="{38372118-311B-4E12-9E8D-1103BB168BE2}">
@@ -501,7 +505,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -534,12 +538,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -909,10 +907,16 @@
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D6" dT="2025-09-21T17:45:02.30" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
-    <text>A comment about a description</text>
+    <text>A comment about a description that becomes a discussion</text>
   </threadedComment>
   <threadedComment ref="D6" dT="2025-09-21T17:45:13.83" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{006CFE16-D608-4ED5-9EA8-037DEA364F8A}" parentId="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
     <text>A threaded reply where there is more infomation</text>
+  </threadedComment>
+  <threadedComment ref="D6" dT="2025-09-24T19:54:53.05" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{5CD65123-C7A5-45B6-9945-CE2F13C8DA05}" parentId="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
+    <text>And continued input for long thread</text>
+  </threadedComment>
+  <threadedComment ref="D6" dT="2025-09-24T19:55:09.26" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{EE427968-BA77-49A5-8C42-8868D7073EBC}" parentId="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
+    <text>This is the end of the discussion</text>
   </threadedComment>
   <threadedComment ref="A12" dT="2025-09-21T17:46:03.58" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{38372118-311B-4E12-9E8D-1103BB168BE2}" done="1">
     <text>A comment that we will marked resolved</text>
@@ -966,7 +970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1064,7 +1070,9 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1657,7 +1665,9 @@
   </sheetPr>
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2400,7 +2410,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2962,7 +2972,7 @@
   </sheetPr>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -5211,6 +5221,267 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
+  <Worksheet>Info</Worksheet>
+  <MapOpenApiRef Row="3">Info./{tenant}/duties/vacant</MapOpenApiRef>
+  <MapOpenApiRef Row="4">Info./{tenant}/duties/{id}</MapOpenApiRef>
+  <MapOpenApiRef Row="5">Info./{tenant}/duties/{id}/split</MapOpenApiRef>
+  <MapOpenApiRef Row="6">Info./{tenant}/duty-assignments</MapOpenApiRef>
+  <MapOpenApiRef Row="7">Info./{tenant}/duty-assignments/{id}/change-cost-centre</MapOpenApiRef>
+  <MapOpenApiRef Row="8">Info./{tenant}/duty-assignments/{id}/grade-override</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>POST_tenant-duty-assignments</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/grade-override.post</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/grade-override.post/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/grade-override.post/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>PUT_tenant-duties-id-split</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}/split.put</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}/split.put/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}/split.put/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}/split.put/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}/split.put/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}/split.put.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}/split.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf</MapOpenApiRef>
+  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}/split.put.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duties/{id}/split.put.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duties/{id}/split.put.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}/split.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}/split.put.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}/split.put.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}/split.put.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}/split.put.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}/split.put.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
   <Worksheet>GET_tenant-duties-vacant</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duties/vacant.get</MapOpenApiRef>
   <MapOpenApiRef Row="5">paths./{tenant}/duties/vacant.get/@path</MapOpenApiRef>
@@ -5378,267 +5649,6 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>PUT_tenant-duties-id-split</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}/split.put</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}/split.put/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}/split.put/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}/split.put/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}/split.put/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}/split.put.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}/split.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf</MapOpenApiRef>
-  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}/split.put.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duties/{id}/split.put.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duties/{id}/split.put.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}/split.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}/split.put.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}/split.put.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}/split.put.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}/split.put.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}/split.put.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>POST_tenant-duty-assignments</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/grade-override.post</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/grade-override.post/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/grade-override.post/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>Info</Worksheet>
-  <MapOpenApiRef Row="3">Info./{tenant}/duties/vacant</MapOpenApiRef>
-  <MapOpenApiRef Row="4">Info./{tenant}/duties/{id}</MapOpenApiRef>
-  <MapOpenApiRef Row="5">Info./{tenant}/duties/{id}/split</MapOpenApiRef>
-  <MapOpenApiRef Row="6">Info./{tenant}/duty-assignments</MapOpenApiRef>
-  <MapOpenApiRef Row="7">Info./{tenant}/duty-assignments/{id}/change-cost-centre</MapOpenApiRef>
-  <MapOpenApiRef Row="8">Info./{tenant}/duty-assignments/{id}/grade-override</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
 <file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>PUT_tenant-duty-assignments-</Worksheet>
@@ -5769,25 +5779,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{712207C2-67E1-4C42-8806-C258C497266D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{127196D2-21C6-4DF6-A4E8-2160E452E096}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB746C33-6FF5-46D6-95F5-9086732ED22F}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C12FDD1-2536-4138-8480-BEAD70AC1FA2}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB746C33-6FF5-46D6-95F5-9086732ED22F}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{127196D2-21C6-4DF6-A4E8-2160E452E096}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{712207C2-67E1-4C42-8806-C258C497266D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Best start to moving migrated comments thus far
</commit_message>
<xml_diff>
--- a/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
+++ b/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\darrenwest-allocate\openapi-2-excel\src\openapi2excel.tests\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920F62B-A3A7-43F5-BDDB-FB2B621CE1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF4F2DA-8650-4495-BB10-FB9DEB89BD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36" yWindow="0" windowWidth="17280" windowHeight="9960" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="GET_tenant-duty-assignments" sheetId="5" r:id="rId5"/>
     <sheet name="PUT_tenant-duty-assignments" sheetId="6" r:id="rId6"/>
     <sheet name="POST_tenant-duty-assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="ROGUE_SHEET" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -177,6 +178,91 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={AC62022F-A443-4F37-A93A-51B6F90BE8AF}</author>
+    <author>tc={3C6A42A2-2676-4989-810E-3EBEC5F5C6D5}</author>
+    <author>tc={4A54003D-2987-41A4-A3E1-B9FBFBBEBB46}</author>
+    <author>tc={66F18A62-4109-4193-9A51-69C5FCBD5056}</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{AC62022F-A443-4F37-A93A-51B6F90BE8AF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Comment no anchor near the top</t>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="1" shapeId="0" xr:uid="{3C6A42A2-2676-4989-810E-3EBEC5F5C6D5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Comment no anchor same row different heading</t>
+      </text>
+    </comment>
+    <comment ref="J35" authorId="2" shapeId="0" xr:uid="{4A54003D-2987-41A4-A3E1-B9FBFBBEBB46}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment with no anchor, below a heading</t>
+      </text>
+    </comment>
+    <comment ref="L35" authorId="3" shapeId="0" xr:uid="{66F18A62-4109-4193-9A51-69C5FCBD5056}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment with no anchor, below a heading
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={77C903D8-C6EF-45FB-83A4-76E87402A1A2}</author>
+    <author>tc={2E742077-2D8B-49ED-9464-23024DF30553}</author>
+    <author>tc={73AD1CE6-0C19-4908-AE58-F20C6D89D9C5}</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{77C903D8-C6EF-45FB-83A4-76E87402A1A2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Comment on a sheet not generated from the open api, and a question seeking reply
+Reply:
+    The reply</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="1" shapeId="0" xr:uid="{2E742077-2D8B-49ED-9464-23024DF30553}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The second rogue comment
+</t>
+      </text>
+    </comment>
+    <comment ref="L12" authorId="2" shapeId="0" xr:uid="{73AD1CE6-0C19-4908-AE58-F20C6D89D9C5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Third rogue comment</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="107">
   <si>
@@ -505,7 +591,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -538,6 +624,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -966,6 +1058,42 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K2" dT="2025-09-26T18:44:49.81" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{AC62022F-A443-4F37-A93A-51B6F90BE8AF}">
+    <text>Comment no anchor near the top</text>
+  </threadedComment>
+  <threadedComment ref="J20" dT="2025-09-26T18:44:22.74" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{3C6A42A2-2676-4989-810E-3EBEC5F5C6D5}">
+    <text>Comment no anchor same row different heading</text>
+  </threadedComment>
+  <threadedComment ref="J35" dT="2025-09-26T18:42:18.01" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{4A54003D-2987-41A4-A3E1-B9FBFBBEBB46}">
+    <text>A comment with no anchor, below a heading</text>
+  </threadedComment>
+  <threadedComment ref="L35" dT="2025-09-26T18:44:02.64" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{66F18A62-4109-4193-9A51-69C5FCBD5056}">
+    <text xml:space="preserve">A comment with no anchor, below a heading
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment7.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D5" dT="2025-09-26T18:31:42.32" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{77C903D8-C6EF-45FB-83A4-76E87402A1A2}">
+    <text>Comment on a sheet not generated from the open api, and a question seeking reply</text>
+  </threadedComment>
+  <threadedComment ref="D5" dT="2025-09-26T18:32:03.01" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{32846916-1922-40AE-9FA2-E5E0DF657D74}" parentId="{77C903D8-C6EF-45FB-83A4-76E87402A1A2}">
+    <text>The reply</text>
+  </threadedComment>
+  <threadedComment ref="H7" dT="2025-09-26T18:41:15.31" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{2E742077-2D8B-49ED-9464-23024DF30553}">
+    <text xml:space="preserve">The second rogue comment
+</text>
+  </threadedComment>
+  <threadedComment ref="L12" dT="2025-09-26T18:41:34.14" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{73AD1CE6-0C19-4908-AE58-F20C6D89D9C5}">
+    <text>Third rogue comment</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
@@ -1070,7 +1198,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3726,13 +3854,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3749,6 +3879,7 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
@@ -4041,6 +4172,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>46</v>
@@ -4242,11 +4374,13 @@
       </c>
     </row>
     <row r="32" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="10:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="'Info'!A1" display="&lt;&lt;&lt;&lt;&lt;" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4775,7 +4909,402 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8EEBBD-512B-418E-B5F2-6D9D78B9C761}">
+  <dimension ref="D5:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>GET_tenant-duties-vacant</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duties/vacant.get</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duties/vacant.get/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duties/vacant.get/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duties/vacant.get/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duties/vacant.get/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.resourcingOrgUnitId</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.resourcingOrgUnitId/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.resourcingOrgUnitId/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.resourcingOrgUnitId/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.resourcingOrgUnitId/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.resourcingOrgUnitId/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.resourcingOrgUnitId/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.resourcingOrgUnitId/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.resourcingOrgUnitId/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.resourcingOrgUnitId/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.resourcingOrgUnitId/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.resourcingOrgUnitId/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.resourcingOrgUnitId/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.resourcingOrgUnitId/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.resourcingOrgUnitId/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.resourcingOrgUnitId/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.resourcingOrgUnitId/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="14">components.parameters.fromDate</MapOpenApiRef>
+  <MapOpenApiRef Cell="A14">components.parameters.fromDate/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C14">components.parameters.fromDate/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D14">components.parameters.fromDate/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E14">components.parameters.fromDate/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F14">components.parameters.fromDate/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G14">components.parameters.fromDate/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H14">components.parameters.fromDate/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I14">components.parameters.fromDate/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J14">components.parameters.fromDate/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K14">components.parameters.fromDate/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L14">components.parameters.fromDate/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M14">components.parameters.fromDate/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N14">components.parameters.fromDate/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O14">components.parameters.fromDate/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P14">components.parameters.fromDate/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q14">components.parameters.fromDate/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters.toDate</MapOpenApiRef>
+  <MapOpenApiRef Cell="A15">components.parameters.toDate/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C15">components.parameters.toDate/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D15">components.parameters.toDate/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E15">components.parameters.toDate/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F15">components.parameters.toDate/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G15">components.parameters.toDate/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H15">components.parameters.toDate/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I15">components.parameters.toDate/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J15">components.parameters.toDate/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K15">components.parameters.toDate/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L15">components.parameters.toDate/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M15">components.parameters.toDate/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N15">components.parameters.toDate/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O15">components.parameters.toDate/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P15">components.parameters.toDate/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q15">components.parameters.toDate/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="16">components.parameters.vacantDutyGradeTypeCategoryId</MapOpenApiRef>
+  <MapOpenApiRef Cell="A16">components.parameters.vacantDutyGradeTypeCategoryId/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C16">components.parameters.vacantDutyGradeTypeCategoryId/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D16">components.parameters.vacantDutyGradeTypeCategoryId/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E16">components.parameters.vacantDutyGradeTypeCategoryId/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F16">components.parameters.vacantDutyGradeTypeCategoryId/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G16">components.parameters.vacantDutyGradeTypeCategoryId/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H16">components.parameters.vacantDutyGradeTypeCategoryId/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I16">components.parameters.vacantDutyGradeTypeCategoryId/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J16">components.parameters.vacantDutyGradeTypeCategoryId/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K16">components.parameters.vacantDutyGradeTypeCategoryId/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L16">components.parameters.vacantDutyGradeTypeCategoryId/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M16">components.parameters.vacantDutyGradeTypeCategoryId/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N16">components.parameters.vacantDutyGradeTypeCategoryId/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O16">components.parameters.vacantDutyGradeTypeCategoryId/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P16">components.parameters.vacantDutyGradeTypeCategoryId/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q16">components.parameters.vacantDutyGradeTypeCategoryId/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="17">components.parameters.vacantDutyGradeTypeId</MapOpenApiRef>
+  <MapOpenApiRef Cell="A17">components.parameters.vacantDutyGradeTypeId/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C17">components.parameters.vacantDutyGradeTypeId/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D17">components.parameters.vacantDutyGradeTypeId/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E17">components.parameters.vacantDutyGradeTypeId/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F17">components.parameters.vacantDutyGradeTypeId/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G17">components.parameters.vacantDutyGradeTypeId/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H17">components.parameters.vacantDutyGradeTypeId/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I17">components.parameters.vacantDutyGradeTypeId/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J17">components.parameters.vacantDutyGradeTypeId/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K17">components.parameters.vacantDutyGradeTypeId/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L17">components.parameters.vacantDutyGradeTypeId/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M17">components.parameters.vacantDutyGradeTypeId/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N17">components.parameters.vacantDutyGradeTypeId/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O17">components.parameters.vacantDutyGradeTypeId/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P17">components.parameters.vacantDutyGradeTypeId/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q17">components.parameters.vacantDutyGradeTypeId/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="18">components.parameters.vacantDutyGradeId</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">components.parameters.vacantDutyGradeId/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C18">components.parameters.vacantDutyGradeId/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D18">components.parameters.vacantDutyGradeId/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">components.parameters.vacantDutyGradeId/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">components.parameters.vacantDutyGradeId/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">components.parameters.vacantDutyGradeId/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">components.parameters.vacantDutyGradeId/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">components.parameters.vacantDutyGradeId/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">components.parameters.vacantDutyGradeId/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">components.parameters.vacantDutyGradeId/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">components.parameters.vacantDutyGradeId/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">components.parameters.vacantDutyGradeId/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">components.parameters.vacantDutyGradeId/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">components.parameters.vacantDutyGradeId/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">components.parameters.vacantDutyGradeId/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">components.parameters.vacantDutyGradeId/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="20">paths./{tenant}/duties/vacant.get.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duties/vacant.get.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duties/vacant.get.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duties/vacant.get.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A24">paths./{tenant}/duties/vacant.get.responses.200.duties/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duties/vacant.get.responses.200.duties</MapOpenApiRef>
+  <MapOpenApiRef Cell="E24">paths./{tenant}/duties/vacant.get.responses.200.duties/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F24">paths./{tenant}/duties/vacant.get.responses.200.duties/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G24">paths./{tenant}/duties/vacant.get.responses.200.duties/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H24">paths./{tenant}/duties/vacant.get.responses.200.duties/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I24">paths./{tenant}/duties/vacant.get.responses.200.duties/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J24">paths./{tenant}/duties/vacant.get.responses.200.duties/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K24">paths./{tenant}/duties/vacant.get.responses.200.duties/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L24">paths./{tenant}/duties/vacant.get.responses.200.duties/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M24">paths./{tenant}/duties/vacant.get.responses.200.duties/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N24">paths./{tenant}/duties/vacant.get.responses.200.duties/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O24">paths./{tenant}/duties/vacant.get.responses.200.duties/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P24">paths./{tenant}/duties/vacant.get.responses.200.duties/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q24">paths./{tenant}/duties/vacant.get.responses.200.duties/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duties/vacant.get.responses.200.duties.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duties/vacant.get.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="28">paths./{tenant}/duties/vacant.get.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duties/vacant.get.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>POST_tenant-duties-id</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}.post</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}.post/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}.post/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}.post/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}.post/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}.post.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}.post.requestBody.workerid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}.post.requestBody.gradeid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber</MapOpenApiRef>
+  <MapOpenApiRef Cell="E20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duties/{id}.post.requestBody.agencyid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}.post.requestBody.externalurl</MapOpenApiRef>
+  <MapOpenApiRef Cell="E22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}.post.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}.post.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}.post.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A29">paths./{tenant}/duties/{id}.post.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duties/{id}.post.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E29">paths./{tenant}/duties/{id}.post.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F29">paths./{tenant}/duties/{id}.post.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G29">paths./{tenant}/duties/{id}.post.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H29">paths./{tenant}/duties/{id}.post.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I29">paths./{tenant}/duties/{id}.post.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J29">paths./{tenant}/duties/{id}.post.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K29">paths./{tenant}/duties/{id}.post.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L29">paths./{tenant}/duties/{id}.post.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M29">paths./{tenant}/duties/{id}.post.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N29">paths./{tenant}/duties/{id}.post.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O29">paths./{tenant}/duties/{id}.post.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P29">paths./{tenant}/duties/{id}.post.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q29">paths./{tenant}/duties/{id}.post.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference</MapOpenApiRef>
+  <MapOpenApiRef Cell="E31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A32">paths./{tenant}/duties/{id}.post.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}.post.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E32">paths./{tenant}/duties/{id}.post.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F32">paths./{tenant}/duties/{id}.post.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G32">paths./{tenant}/duties/{id}.post.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H32">paths./{tenant}/duties/{id}.post.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I32">paths./{tenant}/duties/{id}.post.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J32">paths./{tenant}/duties/{id}.post.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K32">paths./{tenant}/duties/{id}.post.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L32">paths./{tenant}/duties/{id}.post.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M32">paths./{tenant}/duties/{id}.post.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N32">paths./{tenant}/duties/{id}.post.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O32">paths./{tenant}/duties/{id}.post.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P32">paths./{tenant}/duties/{id}.post.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q32">paths./{tenant}/duties/{id}.post.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="33">paths./{tenant}/duties/{id}.post.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="35">paths./{tenant}/duties/{id}.post.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="36">paths./{tenant}/duties/{id}.post.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="37">paths./{tenant}/duties/{id}.post.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>GET_tenant-duty-assignments</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments.get</MapOpenApiRef>
@@ -5012,14 +5541,14 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
-  <Worksheet>POST_tenant-duties-id</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}.post</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}.post/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}.post/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}.post/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}.post/@deprecated</MapOpenApiRef>
+  <Worksheet>PUT_tenant-duty-assignments-</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@deprecated</MapOpenApiRef>
   <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
   <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
   <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
@@ -5057,169 +5586,79 @@
   <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
   <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
   <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}.post.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}.post.requestBody.workerid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}.post.requestBody.workerid/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}.post.requestBody.gradeid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}.post.requestBody.gradeid/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber</MapOpenApiRef>
-  <MapOpenApiRef Cell="E20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q20">paths./{tenant}/duties/{id}.post.requestBody.assignmentnumber/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duties/{id}.post.requestBody.agencyid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q21">paths./{tenant}/duties/{id}.post.requestBody.agencyid/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}.post.requestBody.externalurl</MapOpenApiRef>
-  <MapOpenApiRef Cell="E22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q22">paths./{tenant}/duties/{id}.post.requestBody.externalurl/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}.post.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}.post.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}.post.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A29">paths./{tenant}/duties/{id}.post.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duties/{id}.post.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E29">paths./{tenant}/duties/{id}.post.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F29">paths./{tenant}/duties/{id}.post.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G29">paths./{tenant}/duties/{id}.post.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H29">paths./{tenant}/duties/{id}.post.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I29">paths./{tenant}/duties/{id}.post.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J29">paths./{tenant}/duties/{id}.post.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K29">paths./{tenant}/duties/{id}.post.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L29">paths./{tenant}/duties/{id}.post.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M29">paths./{tenant}/duties/{id}.post.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N29">paths./{tenant}/duties/{id}.post.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O29">paths./{tenant}/duties/{id}.post.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P29">paths./{tenant}/duties/{id}.post.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q29">paths./{tenant}/duties/{id}.post.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q30">paths./{tenant}/duties/{id}.post.responses.200.dutyassignmentid/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference</MapOpenApiRef>
-  <MapOpenApiRef Cell="E31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q31">paths./{tenant}/duties/{id}.post.responses.200.bookingreference/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A32">paths./{tenant}/duties/{id}.post.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}.post.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E32">paths./{tenant}/duties/{id}.post.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F32">paths./{tenant}/duties/{id}.post.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G32">paths./{tenant}/duties/{id}.post.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H32">paths./{tenant}/duties/{id}.post.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I32">paths./{tenant}/duties/{id}.post.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J32">paths./{tenant}/duties/{id}.post.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K32">paths./{tenant}/duties/{id}.post.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L32">paths./{tenant}/duties/{id}.post.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M32">paths./{tenant}/duties/{id}.post.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N32">paths./{tenant}/duties/{id}.post.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O32">paths./{tenant}/duties/{id}.post.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P32">paths./{tenant}/duties/{id}.post.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q32">paths./{tenant}/duties/{id}.post.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="33">paths./{tenant}/duties/{id}.post.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q33">paths./{tenant}/duties/{id}.post.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="35">paths./{tenant}/duties/{id}.post.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="36">paths./{tenant}/duties/{id}.post.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="37">paths./{tenant}/duties/{id}.post.responseBody.500</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.500</MapOpenApiRef>
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>Info</Worksheet>
   <MapOpenApiRef Row="3">Info./{tenant}/duties/vacant</MapOpenApiRef>
@@ -5231,7 +5670,7 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>POST_tenant-duty-assignments</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/grade-override.post</MapOpenApiRef>
@@ -5348,7 +5787,7 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>PUT_tenant-duties-id-split</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}/split.put</MapOpenApiRef>
@@ -5480,294 +5919,8 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>GET_tenant-duties-vacant</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duties/vacant.get</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duties/vacant.get/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duties/vacant.get/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duties/vacant.get/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duties/vacant.get/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.resourcingOrgUnitId</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.resourcingOrgUnitId/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.resourcingOrgUnitId/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.resourcingOrgUnitId/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.resourcingOrgUnitId/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.resourcingOrgUnitId/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.resourcingOrgUnitId/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.resourcingOrgUnitId/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.resourcingOrgUnitId/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.resourcingOrgUnitId/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.resourcingOrgUnitId/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.resourcingOrgUnitId/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.resourcingOrgUnitId/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.resourcingOrgUnitId/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.resourcingOrgUnitId/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.resourcingOrgUnitId/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.resourcingOrgUnitId/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="14">components.parameters.fromDate</MapOpenApiRef>
-  <MapOpenApiRef Cell="A14">components.parameters.fromDate/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C14">components.parameters.fromDate/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D14">components.parameters.fromDate/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E14">components.parameters.fromDate/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F14">components.parameters.fromDate/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G14">components.parameters.fromDate/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H14">components.parameters.fromDate/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I14">components.parameters.fromDate/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J14">components.parameters.fromDate/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K14">components.parameters.fromDate/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L14">components.parameters.fromDate/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M14">components.parameters.fromDate/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N14">components.parameters.fromDate/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O14">components.parameters.fromDate/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P14">components.parameters.fromDate/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q14">components.parameters.fromDate/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters.toDate</MapOpenApiRef>
-  <MapOpenApiRef Cell="A15">components.parameters.toDate/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C15">components.parameters.toDate/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D15">components.parameters.toDate/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E15">components.parameters.toDate/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F15">components.parameters.toDate/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G15">components.parameters.toDate/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H15">components.parameters.toDate/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I15">components.parameters.toDate/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J15">components.parameters.toDate/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K15">components.parameters.toDate/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L15">components.parameters.toDate/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M15">components.parameters.toDate/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N15">components.parameters.toDate/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O15">components.parameters.toDate/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P15">components.parameters.toDate/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q15">components.parameters.toDate/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="16">components.parameters.vacantDutyGradeTypeCategoryId</MapOpenApiRef>
-  <MapOpenApiRef Cell="A16">components.parameters.vacantDutyGradeTypeCategoryId/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C16">components.parameters.vacantDutyGradeTypeCategoryId/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D16">components.parameters.vacantDutyGradeTypeCategoryId/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E16">components.parameters.vacantDutyGradeTypeCategoryId/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F16">components.parameters.vacantDutyGradeTypeCategoryId/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G16">components.parameters.vacantDutyGradeTypeCategoryId/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H16">components.parameters.vacantDutyGradeTypeCategoryId/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I16">components.parameters.vacantDutyGradeTypeCategoryId/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J16">components.parameters.vacantDutyGradeTypeCategoryId/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K16">components.parameters.vacantDutyGradeTypeCategoryId/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L16">components.parameters.vacantDutyGradeTypeCategoryId/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M16">components.parameters.vacantDutyGradeTypeCategoryId/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N16">components.parameters.vacantDutyGradeTypeCategoryId/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O16">components.parameters.vacantDutyGradeTypeCategoryId/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P16">components.parameters.vacantDutyGradeTypeCategoryId/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q16">components.parameters.vacantDutyGradeTypeCategoryId/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="17">components.parameters.vacantDutyGradeTypeId</MapOpenApiRef>
-  <MapOpenApiRef Cell="A17">components.parameters.vacantDutyGradeTypeId/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C17">components.parameters.vacantDutyGradeTypeId/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D17">components.parameters.vacantDutyGradeTypeId/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E17">components.parameters.vacantDutyGradeTypeId/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F17">components.parameters.vacantDutyGradeTypeId/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G17">components.parameters.vacantDutyGradeTypeId/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H17">components.parameters.vacantDutyGradeTypeId/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I17">components.parameters.vacantDutyGradeTypeId/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J17">components.parameters.vacantDutyGradeTypeId/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K17">components.parameters.vacantDutyGradeTypeId/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L17">components.parameters.vacantDutyGradeTypeId/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M17">components.parameters.vacantDutyGradeTypeId/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N17">components.parameters.vacantDutyGradeTypeId/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O17">components.parameters.vacantDutyGradeTypeId/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P17">components.parameters.vacantDutyGradeTypeId/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q17">components.parameters.vacantDutyGradeTypeId/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="18">components.parameters.vacantDutyGradeId</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">components.parameters.vacantDutyGradeId/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C18">components.parameters.vacantDutyGradeId/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D18">components.parameters.vacantDutyGradeId/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">components.parameters.vacantDutyGradeId/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">components.parameters.vacantDutyGradeId/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">components.parameters.vacantDutyGradeId/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">components.parameters.vacantDutyGradeId/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">components.parameters.vacantDutyGradeId/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">components.parameters.vacantDutyGradeId/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">components.parameters.vacantDutyGradeId/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">components.parameters.vacantDutyGradeId/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">components.parameters.vacantDutyGradeId/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">components.parameters.vacantDutyGradeId/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">components.parameters.vacantDutyGradeId/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">components.parameters.vacantDutyGradeId/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">components.parameters.vacantDutyGradeId/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="20">paths./{tenant}/duties/vacant.get.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duties/vacant.get.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duties/vacant.get.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duties/vacant.get.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A24">paths./{tenant}/duties/vacant.get.responses.200.duties/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duties/vacant.get.responses.200.duties</MapOpenApiRef>
-  <MapOpenApiRef Cell="E24">paths./{tenant}/duties/vacant.get.responses.200.duties/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F24">paths./{tenant}/duties/vacant.get.responses.200.duties/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G24">paths./{tenant}/duties/vacant.get.responses.200.duties/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H24">paths./{tenant}/duties/vacant.get.responses.200.duties/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I24">paths./{tenant}/duties/vacant.get.responses.200.duties/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J24">paths./{tenant}/duties/vacant.get.responses.200.duties/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K24">paths./{tenant}/duties/vacant.get.responses.200.duties/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L24">paths./{tenant}/duties/vacant.get.responses.200.duties/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M24">paths./{tenant}/duties/vacant.get.responses.200.duties/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N24">paths./{tenant}/duties/vacant.get.responses.200.duties/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O24">paths./{tenant}/duties/vacant.get.responses.200.duties/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P24">paths./{tenant}/duties/vacant.get.responses.200.duties/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q24">paths./{tenant}/duties/vacant.get.responses.200.duties/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duties/vacant.get.responses.200.duties.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q25">paths./{tenant}/duties/vacant.get.responses.200.duties.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duties/vacant.get.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="28">paths./{tenant}/duties/vacant.get.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duties/vacant.get.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>PUT_tenant-duty-assignments-</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDFEBF9-4D51-4C81-A9EB-15C6FCA4D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{712207C2-67E1-4C42-8806-C258C497266D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -5779,31 +5932,31 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDFEBF9-4D51-4C81-A9EB-15C6FCA4D05E}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D2B8F1C-04F9-4A20-9627-A687A53E3335}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{127196D2-21C6-4DF6-A4E8-2160E452E096}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB746C33-6FF5-46D6-95F5-9086732ED22F}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C12FDD1-2536-4138-8480-BEAD70AC1FA2}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{712207C2-67E1-4C42-8806-C258C497266D}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D2B8F1C-04F9-4A20-9627-A687A53E3335}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
NoAnchor Type A migration now working
</commit_message>
<xml_diff>
--- a/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
+++ b/src/openapi2excel.tests/Sample/sample-api-gw-with-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\darrenwest-allocate\openapi-2-excel\src\openapi2excel.tests\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF4F2DA-8650-4495-BB10-FB9DEB89BD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE174A29-25CE-453E-BB46-D449BE78D8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="0" windowWidth="17280" windowHeight="9960" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="POST_tenant-duties-id" sheetId="3" r:id="rId3"/>
     <sheet name="PUT_tenant-duties-id-split" sheetId="4" r:id="rId4"/>
     <sheet name="GET_tenant-duty-assignments" sheetId="5" r:id="rId5"/>
-    <sheet name="PUT_tenant-duty-assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="PUT_tenant-duty-assignments-" sheetId="6" r:id="rId6"/>
     <sheet name="POST_tenant-duty-assignments" sheetId="7" r:id="rId7"/>
     <sheet name="ROGUE_SHEET" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -200,7 +200,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Comment no anchor same row different heading</t>
+    Comment no anchor same row different heading, below the REQUEST titlerow</t>
       </text>
     </comment>
     <comment ref="J35" authorId="2" shapeId="0" xr:uid="{4A54003D-2987-41A4-A3E1-B9FBFBBEBB46}">
@@ -208,16 +208,17 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    A comment with no anchor, below a heading</t>
+    A comment with no anchor, below the RESPONSE title row</t>
       </text>
     </comment>
     <comment ref="L35" authorId="3" shapeId="0" xr:uid="{66F18A62-4109-4193-9A51-69C5FCBD5056}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    A comment with no anchor, below a heading
-</t>
+    A comment with no anchor, below a heading in column L that has a reply
+Reply:
+    I am replying to the comment of column L</t>
       </text>
     </comment>
   </commentList>
@@ -591,7 +592,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -624,12 +625,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1064,14 +1059,17 @@
     <text>Comment no anchor near the top</text>
   </threadedComment>
   <threadedComment ref="J20" dT="2025-09-26T18:44:22.74" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{3C6A42A2-2676-4989-810E-3EBEC5F5C6D5}">
-    <text>Comment no anchor same row different heading</text>
+    <text>Comment no anchor same row different heading, below the REQUEST titlerow</text>
   </threadedComment>
   <threadedComment ref="J35" dT="2025-09-26T18:42:18.01" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{4A54003D-2987-41A4-A3E1-B9FBFBBEBB46}">
-    <text>A comment with no anchor, below a heading</text>
+    <text>A comment with no anchor, below the RESPONSE title row</text>
   </threadedComment>
   <threadedComment ref="L35" dT="2025-09-26T18:44:02.64" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{66F18A62-4109-4193-9A51-69C5FCBD5056}">
-    <text xml:space="preserve">A comment with no anchor, below a heading
+    <text xml:space="preserve">A comment with no anchor, below a heading in column L that has a reply
 </text>
+  </threadedComment>
+  <threadedComment ref="L35" dT="2025-09-28T02:20:39.69" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{A91B4098-39E1-467F-A8BD-4F2946E203A1}" parentId="{66F18A62-4109-4193-9A51-69C5FCBD5056}">
+    <text>I am replying to the comment of column L</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -3101,7 +3099,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -3860,8 +3858,8 @@
   </sheetPr>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -4929,6 +4927,123 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>PUT_tenant-duty-assignments-</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>GET_tenant-duties-vacant</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duties/vacant.get</MapOpenApiRef>
@@ -5097,7 +5212,136 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>Info</Worksheet>
+  <MapOpenApiRef Row="3">Info./{tenant}/duties/vacant</MapOpenApiRef>
+  <MapOpenApiRef Row="4">Info./{tenant}/duties/{id}</MapOpenApiRef>
+  <MapOpenApiRef Row="5">Info./{tenant}/duties/{id}/split</MapOpenApiRef>
+  <MapOpenApiRef Row="6">Info./{tenant}/duty-assignments</MapOpenApiRef>
+  <MapOpenApiRef Row="7">Info./{tenant}/duty-assignments/{id}/change-cost-centre</MapOpenApiRef>
+  <MapOpenApiRef Row="8">Info./{tenant}/duty-assignments/{id}/grade-override</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>POST_tenant-duty-assignments</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/grade-override.post</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/grade-override.post/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/grade-override.post/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>POST_tenant-duties-id</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}.post</MapOpenApiRef>
@@ -5304,7 +5548,139 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<OpenApiMappings>
+  <Worksheet>PUT_tenant-duties-id-split</Worksheet>
+  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}/split.put</MapOpenApiRef>
+  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}/split.put/@path</MapOpenApiRef>
+  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}/split.put/@operation_description</MapOpenApiRef>
+  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}/split.put/@operation_summary</MapOpenApiRef>
+  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}/split.put/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
+  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
+  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
+  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
+  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
+  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
+  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
+  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
+  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}/split.put.requestBody/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}/split.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset</MapOpenApiRef>
+  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf</MapOpenApiRef>
+  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}/split.put.responseBody</MapOpenApiRef>
+  <MapOpenApiRef Row="23">paths./{tenant}/duties/{id}/split.put.responseBody.200</MapOpenApiRef>
+  <MapOpenApiRef Row="24">paths./{tenant}/duties/{id}/split.put.responses.200/@bodyformat</MapOpenApiRef>
+  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}/split.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
+  <MapOpenApiRef Cell="A26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}/split.put.responses.200.success</MapOpenApiRef>
+  <MapOpenApiRef Cell="E26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="A27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}/split.put.responses.200.errors</MapOpenApiRef>
+  <MapOpenApiRef Cell="E27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@description</MapOpenApiRef>
+  <MapOpenApiRef Cell="B28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@name</MapOpenApiRef>
+  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value</MapOpenApiRef>
+  <MapOpenApiRef Cell="E28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@type</MapOpenApiRef>
+  <MapOpenApiRef Cell="F28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
+  <MapOpenApiRef Cell="G28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@format</MapOpenApiRef>
+  <MapOpenApiRef Cell="H28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@length</MapOpenApiRef>
+  <MapOpenApiRef Cell="I28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@required</MapOpenApiRef>
+  <MapOpenApiRef Cell="J28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@nullable</MapOpenApiRef>
+  <MapOpenApiRef Cell="K28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@range</MapOpenApiRef>
+  <MapOpenApiRef Cell="L28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@pattern</MapOpenApiRef>
+  <MapOpenApiRef Cell="M28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@enum</MapOpenApiRef>
+  <MapOpenApiRef Cell="N28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
+  <MapOpenApiRef Cell="O28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@default</MapOpenApiRef>
+  <MapOpenApiRef Cell="P28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@example</MapOpenApiRef>
+  <MapOpenApiRef Cell="Q28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@description</MapOpenApiRef>
+  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}/split.put.responseBody.400</MapOpenApiRef>
+  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}/split.put.responseBody.404</MapOpenApiRef>
+  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}/split.put.responseBody.500</MapOpenApiRef>
+</OpenApiMappings>
+</file>
+
+<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
 <OpenApiMappings>
   <Worksheet>GET_tenant-duty-assignments</Worksheet>
   <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments.get</MapOpenApiRef>
@@ -5541,422 +5917,44 @@
 </OpenApiMappings>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>PUT_tenant-duty-assignments-</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.requestBody.costcentreid/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/change-cost-centre.put.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D2B8F1C-04F9-4A20-9627-A687A53E3335}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>Info</Worksheet>
-  <MapOpenApiRef Row="3">Info./{tenant}/duties/vacant</MapOpenApiRef>
-  <MapOpenApiRef Row="4">Info./{tenant}/duties/{id}</MapOpenApiRef>
-  <MapOpenApiRef Row="5">Info./{tenant}/duties/{id}/split</MapOpenApiRef>
-  <MapOpenApiRef Row="6">Info./{tenant}/duty-assignments</MapOpenApiRef>
-  <MapOpenApiRef Row="7">Info./{tenant}/duty-assignments/{id}/change-cost-centre</MapOpenApiRef>
-  <MapOpenApiRef Row="8">Info./{tenant}/duty-assignments/{id}/grade-override</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>POST_tenant-duty-assignments</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duty-assignments/{id}/grade-override.post</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duty-assignments/{id}/grade-override.post/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duty-assignments/{id}/grade-override.post/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duty-assignments/{id}/grade-override.post/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duty-assignments/{id}/grade-override.post.requestBody.gradeid/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="21">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q25">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duty-assignments/{id}/grade-override.post.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="29">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duty-assignments/{id}/grade-override.post.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
-<OpenApiMappings>
-  <Worksheet>PUT_tenant-duties-id-split</Worksheet>
-  <MapOpenApiRef Row="4">paths./{tenant}/duties/{id}/split.put</MapOpenApiRef>
-  <MapOpenApiRef Row="5">paths./{tenant}/duties/{id}/split.put/@path</MapOpenApiRef>
-  <MapOpenApiRef Row="6">paths./{tenant}/duties/{id}/split.put/@operation_description</MapOpenApiRef>
-  <MapOpenApiRef Row="7">paths./{tenant}/duties/{id}/split.put/@operation_summary</MapOpenApiRef>
-  <MapOpenApiRef Row="8">paths./{tenant}/duties/{id}/split.put/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Row="10">components.parameters./Title</MapOpenApiRef>
-  <MapOpenApiRef Row="11">components.parameters./ParameterHeadings</MapOpenApiRef>
-  <MapOpenApiRef Row="12">components.parameters.tenant</MapOpenApiRef>
-  <MapOpenApiRef Cell="A12">components.parameters.tenant/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C12">components.parameters.tenant/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D12">components.parameters.tenant/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E12">components.parameters.tenant/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F12">components.parameters.tenant/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G12">components.parameters.tenant/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H12">components.parameters.tenant/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I12">components.parameters.tenant/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J12">components.parameters.tenant/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K12">components.parameters.tenant/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L12">components.parameters.tenant/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M12">components.parameters.tenant/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N12">components.parameters.tenant/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O12">components.parameters.tenant/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P12">components.parameters.tenant/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q12">components.parameters.tenant/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="13">components.parameters.id</MapOpenApiRef>
-  <MapOpenApiRef Cell="A13">components.parameters.id/@name</MapOpenApiRef>
-  <MapOpenApiRef Cell="C13">components.parameters.id/@location</MapOpenApiRef>
-  <MapOpenApiRef Cell="D13">components.parameters.id/@serialization</MapOpenApiRef>
-  <MapOpenApiRef Cell="E13">components.parameters.id/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F13">components.parameters.id/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G13">components.parameters.id/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H13">components.parameters.id/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I13">components.parameters.id/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J13">components.parameters.id/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K13">components.parameters.id/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L13">components.parameters.id/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M13">components.parameters.id/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N13">components.parameters.id/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O13">components.parameters.id/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P13">components.parameters.id/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q13">components.parameters.id/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="15">components.parameters./Title/@request</MapOpenApiRef>
-  <MapOpenApiRef Row="16">paths./{tenant}/duties/{id}/split.put.requestBody/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="17">paths./{tenant}/duties/{id}/split.put.requestBody/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset</MapOpenApiRef>
-  <MapOpenApiRef Cell="E18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q18">paths./{tenant}/duties/{id}/split.put.requestBody.splitoffset/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf</MapOpenApiRef>
-  <MapOpenApiRef Cell="E19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q19">paths./{tenant}/duties/{id}/split.put.requestBody.stubfirsthalf/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="22">paths./{tenant}/duties/{id}/split.put.responseBody</MapOpenApiRef>
-  <MapOpenApiRef Row="23">paths./{tenant}/duties/{id}/split.put.responseBody.200</MapOpenApiRef>
-  <MapOpenApiRef Row="24">paths./{tenant}/duties/{id}/split.put.responses.200/@bodyformat</MapOpenApiRef>
-  <MapOpenApiRef Row="25">paths./{tenant}/duties/{id}/split.put.responses.200/SchemaDescriptionHeader</MapOpenApiRef>
-  <MapOpenApiRef Cell="A26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="26">paths./{tenant}/duties/{id}/split.put.responses.200.success</MapOpenApiRef>
-  <MapOpenApiRef Cell="E26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q26">paths./{tenant}/duties/{id}/split.put.responses.200.success/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="A27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="27">paths./{tenant}/duties/{id}/split.put.responses.200.errors</MapOpenApiRef>
-  <MapOpenApiRef Cell="E27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q27">paths./{tenant}/duties/{id}/split.put.responses.200.errors/@description</MapOpenApiRef>
-  <MapOpenApiRef Cell="B28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@name</MapOpenApiRef>
-  <MapOpenApiRef Row="28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value</MapOpenApiRef>
-  <MapOpenApiRef Cell="E28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@type</MapOpenApiRef>
-  <MapOpenApiRef Cell="F28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@objecttype</MapOpenApiRef>
-  <MapOpenApiRef Cell="G28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@format</MapOpenApiRef>
-  <MapOpenApiRef Cell="H28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@length</MapOpenApiRef>
-  <MapOpenApiRef Cell="I28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@required</MapOpenApiRef>
-  <MapOpenApiRef Cell="J28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@nullable</MapOpenApiRef>
-  <MapOpenApiRef Cell="K28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@range</MapOpenApiRef>
-  <MapOpenApiRef Cell="L28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@pattern</MapOpenApiRef>
-  <MapOpenApiRef Cell="M28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@enum</MapOpenApiRef>
-  <MapOpenApiRef Cell="N28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@deprecated</MapOpenApiRef>
-  <MapOpenApiRef Cell="O28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@default</MapOpenApiRef>
-  <MapOpenApiRef Cell="P28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@example</MapOpenApiRef>
-  <MapOpenApiRef Cell="Q28">paths./{tenant}/duties/{id}/split.put.responses.200.errors.value/@description</MapOpenApiRef>
-  <MapOpenApiRef Row="30">paths./{tenant}/duties/{id}/split.put.responseBody.400</MapOpenApiRef>
-  <MapOpenApiRef Row="31">paths./{tenant}/duties/{id}/split.put.responseBody.404</MapOpenApiRef>
-  <MapOpenApiRef Row="32">paths./{tenant}/duties/{id}/split.put.responseBody.500</MapOpenApiRef>
-</OpenApiMappings>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{712207C2-67E1-4C42-8806-C258C497266D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{127196D2-21C6-4DF6-A4E8-2160E452E096}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB746C33-6FF5-46D6-95F5-9086732ED22F}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D84D8F45-DB52-4C6F-A2DE-7E3A11FFB091}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDFEBF9-4D51-4C81-A9EB-15C6FCA4D05E}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D2B8F1C-04F9-4A20-9627-A687A53E3335}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{127196D2-21C6-4DF6-A4E8-2160E452E096}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB746C33-6FF5-46D6-95F5-9086732ED22F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C12FDD1-2536-4138-8480-BEAD70AC1FA2}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C12FDD1-2536-4138-8480-BEAD70AC1FA2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDFEBF9-4D51-4C81-A9EB-15C6FCA4D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>